<commit_message>
Test Cases Are added
</commit_message>
<xml_diff>
--- a/WIXWAVITYPROJECT/TestData.xlsx
+++ b/WIXWAVITYPROJECT/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="PollsData" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,12 @@
     <sheet name="NewType" sheetId="3" r:id="rId3"/>
     <sheet name="NewAppSheet" sheetId="4" r:id="rId4"/>
     <sheet name="CreateAnAppWithTextNumber" sheetId="7" r:id="rId5"/>
-    <sheet name="CreateAnAppWithNumbers" sheetId="8" r:id="rId6"/>
+    <sheet name="CreateAnAppWithNumbers" sheetId="10" r:id="rId6"/>
+    <sheet name="CreateAnAppWithCategory" sheetId="8" r:id="rId7"/>
+    <sheet name="CreateAnAppWithDependents" sheetId="11" r:id="rId8"/>
+    <sheet name="CreateAnAppWithReference" sheetId="12" r:id="rId9"/>
+    <sheet name="CreateAnAppWithProgress" sheetId="13" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="295">
   <si>
     <t>PollName</t>
   </si>
@@ -605,12 +610,6 @@
     <t>I am Test Engineer</t>
   </si>
   <si>
-    <t>I am Railway police</t>
-  </si>
-  <si>
-    <t>I am Friend</t>
-  </si>
-  <si>
     <t>CA Guy</t>
   </si>
   <si>
@@ -722,19 +721,10 @@
     <t>http://tenant42.wavity.info;2YEARS;WAVITY</t>
   </si>
   <si>
-    <t>http://we.wavity.com;1YEAR;RAILWAYS</t>
-  </si>
-  <si>
     <t>http://abc.com;4YEARS;RxCurrencyExchange</t>
   </si>
   <si>
     <t>http://gmail.com;4YEARS;CA National</t>
-  </si>
-  <si>
-    <t>WIX_WAVE_TEXT_CONTROL_APP</t>
-  </si>
-  <si>
-    <t>WIX_WAVE_NUMBERS_CONTROL_APP</t>
   </si>
   <si>
     <t>Creating An App with Numbers Control</t>
@@ -778,6 +768,154 @@
   <si>
     <t xml:space="preserve">Required;Deprecated;Required;Read only;Read only;Help message:Trying To Select All The Properties;Scale:8;Allow negative;Placeholder:Checking All Properties For One Control;Default value:1200.56789876 ;Populate on create;Allow data import;Font size:32;Font weight:Light;Font style:Normal;One time entry
 </t>
+  </si>
+  <si>
+    <t>Font size: 32</t>
+  </si>
+  <si>
+    <t>Suffix: Vivek</t>
+  </si>
+  <si>
+    <t>Akon often provides vocals as a featured artist and is currently credited with over 300 guest appearances and more than 35 Billboard Hot 100 songs, resulting in five Grammy Awards nominations. He has released six solo albums and has handled the majority of production on his solo work and guest features. Alongside this, he also produced records mainly for artists on his respective labels, as well as for other artists such as Michael Jackson, Snoop Dogg, Lionel Richie, Leona Lewis, Sean Paul and Whitney Houston.
+Forbes ranked Akon 80th (Power Rank) in Forbes Celebrity 100 in 2010[4] and 5th in 40 Most Powerful Celebrities in Africa list, in 2011.[5] Billboard ranked Akon No. 6 on the list of Top Digital Songs Artists of the decade.[6]</t>
+  </si>
+  <si>
+    <t>Kina Cosper (born January 25, 1969) is an American musician, best known for her work with Grammy Award-nominated group Brownstone (after their nomination), and her 2000 solo single "Girl from the Gutter".</t>
+  </si>
+  <si>
+    <t>http://abc.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At 16 years old, Bieber released his debut studio album My World 2.0 (2010), which contained the hit single "Baby". The album debuted atop the US Billboard 200, making Bieber the youngest solo male act to top the chart in 47 years.[7] Bieber had quickly established himself as a teen idol.[8] Following his debut album and promotional tours, he released his 3D biopic-concert film Justin Bieber: Never Say Never, which was a box office success. Bieber's next album, Under the Mistletoe (2011), became the first Christmas album by a male artist to debut at number one on the Billboard 200.[9] In the years following the release of Believe (2012), Bieber faced several controversies for his rebellious nature, including run-ins with the law internationally.[10] "Where Are Ü Now", a collaboration with Skrillex and Diplo released in 2015, marked a new era of Bieber's career,[11] as he transitioned into EDM and moved away from teen pop.[12] </t>
+  </si>
+  <si>
+    <t>Wix_Text_Control_App</t>
+  </si>
+  <si>
+    <t>Wix_Category_Control_App</t>
+  </si>
+  <si>
+    <t>Wix_Numbers_Control_App</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Control Objects</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>Value:Vive211;Value:Shan212;Value:Mla12;Display Name:211; Display Name: 212; Display Name:12</t>
+  </si>
+  <si>
+    <t>Value:Vive211;Value:Shan212;Value:Mla12;Display Name:211; Display Name: 212; Display Name:13</t>
+  </si>
+  <si>
+    <t>Value:Vive211;Value:Shan212;Value:Mla12;Display Name:211; Display Name: 212; Display Name:14</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>211;Other:VivekReddyM;12</t>
+  </si>
+  <si>
+    <t>Required ;Selection type:Multiple;Min selection:1;Max selection:3;option while record entry</t>
+  </si>
+  <si>
+    <t>Help message: I am Checking;option while record entry;Selection:Multiple;Min selection:1;Max selection:3;</t>
+  </si>
+  <si>
+    <t>Other:Nanda;211;212</t>
+  </si>
+  <si>
+    <t>Other:XNTOX;13</t>
+  </si>
+  <si>
+    <t>Dependent</t>
+  </si>
+  <si>
+    <t>Wix_Dependent_Control_App</t>
+  </si>
+  <si>
+    <t>Creating An App with Dependents Control</t>
+  </si>
+  <si>
+    <t>Application:SampleApp;   Value from:text;     Match:text;    With:text</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Help message:As a mach for dependent</t>
+  </si>
+  <si>
+    <t>Help message:I am Checking</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Category Dependent1</t>
+  </si>
+  <si>
+    <t>Category Dependent2</t>
+  </si>
+  <si>
+    <t>Category Dependent3</t>
+  </si>
+  <si>
+    <t>Application:SampleApp;   Value from:text;     Match:number;    With:number</t>
+  </si>
+  <si>
+    <t>Application:SampleApp;   Value from:text;     Match:date;    With:date</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Application:SampleApp;   Value:text;     Display Name:text</t>
+  </si>
+  <si>
+    <t>Category Reference1</t>
+  </si>
+  <si>
+    <t>Category Reference2</t>
+  </si>
+  <si>
+    <t>Dependent Multi Values</t>
+  </si>
+  <si>
+    <t>Category Dependent Multi Values</t>
+  </si>
+  <si>
+    <t>Depends On:text;   Application:SampleApp;  Match:text;  Value(s) from:text; Value(s) from:number</t>
+  </si>
+  <si>
+    <t>Font Size:20</t>
+  </si>
+  <si>
+    <t>Toggle</t>
+  </si>
+  <si>
+    <t>Creating An App with Progress Control</t>
+  </si>
+  <si>
+    <t>Collaboration</t>
+  </si>
+  <si>
+    <t>Wix_Progress_Control_App</t>
+  </si>
+  <si>
+    <t>Help message: I am Checking Sliders</t>
   </si>
 </sst>
 </file>
@@ -919,7 +1057,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1000,7 +1138,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1013,6 +1150,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1415,6 +1571,288 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="4" width="35.85546875" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" style="67" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>291</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>292</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>291</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>291</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+    </row>
+    <row r="7" spans="1:12" ht="18.75" customHeight="1">
+      <c r="A7" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1">
+      <c r="A8" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="G8" s="42">
+        <v>212</v>
+      </c>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
@@ -3486,7 +3924,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3496,7 +3934,7 @@
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="35.7109375" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="6" max="6" width="54.140625" style="67" customWidth="1"/>
     <col min="7" max="7" width="30.42578125" customWidth="1"/>
     <col min="8" max="8" width="41.7109375" customWidth="1"/>
     <col min="9" max="9" width="33.5703125" customWidth="1"/>
@@ -3520,7 +3958,7 @@
       <c r="E1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="27"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
       <c r="I1" s="27"/>
@@ -3536,7 +3974,7 @@
         <v>93</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>39</v>
@@ -3544,7 +3982,7 @@
       <c r="E2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="27"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="27"/>
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
@@ -3560,7 +3998,7 @@
         <v>92</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>39</v>
@@ -3568,7 +4006,7 @@
       <c r="E3" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="27"/>
+      <c r="F3" s="36"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
@@ -3584,7 +4022,7 @@
         <v>94</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>39</v>
@@ -3592,7 +4030,7 @@
       <c r="E4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="27"/>
+      <c r="F4" s="36"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
       <c r="I4" s="27"/>
@@ -3608,7 +4046,7 @@
         <v>95</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
       <c r="D5" s="30" t="s">
         <v>39</v>
@@ -3616,7 +4054,7 @@
       <c r="E5" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
       <c r="I5" s="27"/>
@@ -3630,7 +4068,7 @@
       <c r="C6" s="31"/>
       <c r="D6" s="32"/>
       <c r="E6" s="31"/>
-      <c r="F6" s="27"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="27"/>
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
@@ -3654,7 +4092,7 @@
       <c r="E7" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="64" t="s">
         <v>180</v>
       </c>
       <c r="G7" s="25" t="s">
@@ -3670,10 +4108,10 @@
         <v>184</v>
       </c>
       <c r="K7" s="25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L7" s="25" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -3692,7 +4130,7 @@
       <c r="E8" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="36" t="s">
         <v>105</v>
       </c>
       <c r="G8" s="27" t="s">
@@ -3714,7 +4152,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" ht="48.75" customHeight="1">
       <c r="A9" s="28" t="s">
         <v>31</v>
       </c>
@@ -3728,25 +4166,25 @@
         <v>189</v>
       </c>
       <c r="E9" s="60" t="s">
-        <v>228</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="G9" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="I9" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="J9" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="I9" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="J9" s="27" t="s">
-        <v>196</v>
-      </c>
       <c r="K9" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L9" s="27" t="s">
         <v>192</v>
@@ -3766,28 +4204,28 @@
         <v>190</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>229</v>
-      </c>
-      <c r="F10" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="H10" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="I10" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="J10" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="I10" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="J10" s="27" t="s">
-        <v>201</v>
-      </c>
       <c r="K10" s="27" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L10" s="27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -3804,28 +4242,28 @@
         <v>191</v>
       </c>
       <c r="E11" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="G11" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="H11" s="48" t="s">
         <v>230</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="I11" s="27" t="s">
         <v>231</v>
       </c>
-      <c r="G11" s="48" t="s">
-        <v>232</v>
-      </c>
-      <c r="H11" s="48" t="s">
-        <v>233</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>234</v>
-      </c>
       <c r="J11" s="27" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L11" s="27" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -3841,14 +4279,16 @@
       <c r="D12" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="62"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
+      <c r="E12" s="61" t="s">
+        <v>246</v>
+      </c>
+      <c r="F12" s="68"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
       <c r="K12" s="27"/>
-      <c r="L12" s="63"/>
+      <c r="L12" s="62"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="28" t="s">
@@ -3863,34 +4303,36 @@
       <c r="D13" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="E13" s="62"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
+      <c r="E13" s="61" t="s">
+        <v>247</v>
+      </c>
+      <c r="F13" s="68"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
       <c r="K13" s="27"/>
-      <c r="L13" s="63"/>
+      <c r="L13" s="62"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="64"/>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
+      <c r="A14" s="63"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F11" r:id="rId1"/>
-    <hyperlink ref="G11" r:id="rId2"/>
-    <hyperlink ref="H11" r:id="rId3"/>
+    <hyperlink ref="H11" r:id="rId2"/>
+    <hyperlink ref="G11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -3901,8 +4343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3910,7 +4352,7 @@
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" customWidth="1"/>
     <col min="3" max="4" width="35.85546875" customWidth="1"/>
-    <col min="5" max="5" width="51.140625" style="68" customWidth="1"/>
+    <col min="5" max="5" width="51.140625" style="67" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
@@ -3933,7 +4375,7 @@
       <c r="D1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="64" t="s">
         <v>29</v>
       </c>
       <c r="F1" s="27"/>
@@ -3952,10 +4394,10 @@
         <v>93</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>236</v>
+        <v>253</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E2" s="36" t="s">
         <v>34</v>
@@ -3976,10 +4418,10 @@
         <v>92</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>236</v>
+        <v>253</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E3" s="36" t="s">
         <v>35</v>
@@ -4000,10 +4442,10 @@
         <v>94</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>236</v>
+        <v>253</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E4" s="36" t="s">
         <v>36</v>
@@ -4024,10 +4466,10 @@
         <v>95</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>236</v>
+        <v>253</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E5" s="36" t="s">
         <v>37</v>
@@ -4045,7 +4487,7 @@
       <c r="B6" s="31"/>
       <c r="C6" s="31"/>
       <c r="D6" s="32"/>
-      <c r="E6" s="66"/>
+      <c r="E6" s="65"/>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
       <c r="H6" s="27"/>
@@ -4067,7 +4509,7 @@
       <c r="D7" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="64" t="s">
         <v>177</v>
       </c>
       <c r="F7" s="25" t="s">
@@ -4086,10 +4528,10 @@
         <v>184</v>
       </c>
       <c r="K7" s="25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L7" s="25" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="75.75" customHeight="1">
@@ -4103,10 +4545,10 @@
         <v>83</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F8" s="42" t="s">
         <v>31</v>
@@ -4141,28 +4583,28 @@
         <v>83</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F9" s="42" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G9" s="42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H9" s="42" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I9" s="42" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J9" s="42" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K9" s="42" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L9" s="42" t="s">
         <v>162</v>
@@ -4179,28 +4621,28 @@
         <v>138</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F10" s="42" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H10" s="42" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I10" s="42" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J10" s="42" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K10" s="42" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="L10" s="42" t="s">
         <v>163</v>
@@ -4217,28 +4659,28 @@
         <v>138</v>
       </c>
       <c r="D11" s="61" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H11" s="42" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I11" s="42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J11" s="42" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K11" s="42" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L11" s="42" t="s">
         <v>164</v>
@@ -4255,48 +4697,1237 @@
         <v>83</v>
       </c>
       <c r="D12" s="61" t="s">
+        <v>233</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>234</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="H12" s="42" t="s">
+        <v>236</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="J12" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="E12" s="36" t="s">
-        <v>249</v>
-      </c>
-      <c r="F12" s="42" t="s">
+      <c r="K12" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="G12" s="42" t="s">
+      <c r="L12" s="42" t="s">
         <v>240</v>
       </c>
-      <c r="H12" s="42" t="s">
-        <v>241</v>
-      </c>
-      <c r="I12" s="42" t="s">
-        <v>242</v>
-      </c>
-      <c r="J12" s="42" t="s">
-        <v>243</v>
-      </c>
-      <c r="K12" s="42" t="s">
-        <v>244</v>
-      </c>
-      <c r="L12" s="42" t="s">
-        <v>245</v>
-      </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="64"/>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="64"/>
+      <c r="A13" s="63"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="4" width="35.85546875" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" style="67" customWidth="1"/>
+    <col min="6" max="6" width="51.140625" style="67" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" customWidth="1"/>
+    <col min="11" max="11" width="8" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+    </row>
+    <row r="7" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A7" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="64" t="s">
+        <v>256</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="49.5" customHeight="1">
+      <c r="A8" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="H8" s="42">
+        <v>212</v>
+      </c>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+    </row>
+    <row r="9" spans="1:13" ht="39">
+      <c r="A9" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+    </row>
+    <row r="10" spans="1:13" ht="26.25">
+      <c r="A10" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>262</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>260</v>
+      </c>
+      <c r="G10" s="27">
+        <v>14</v>
+      </c>
+      <c r="H10" s="42">
+        <v>14</v>
+      </c>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="63"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="4" width="35.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" style="67" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" style="67" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" customWidth="1"/>
+    <col min="11" max="11" width="8" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+    </row>
+    <row r="7" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A7" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="64" t="s">
+        <v>256</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="72" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A8" s="73" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="F8" s="38"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+    </row>
+    <row r="9" spans="1:13" s="72" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A9" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="61" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="F9" s="38"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+    </row>
+    <row r="10" spans="1:13" s="72" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A10" s="73" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="F10" s="38"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+    </row>
+    <row r="11" spans="1:13" ht="30.75" customHeight="1">
+      <c r="A11" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="H11" s="42">
+        <v>212</v>
+      </c>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+    </row>
+    <row r="12" spans="1:13" ht="26.25">
+      <c r="A12" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+    </row>
+    <row r="13" spans="1:13" ht="26.25">
+      <c r="A13" s="73" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>281</v>
+      </c>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="63"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="63"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="4" width="35.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" style="67" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" style="67" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" customWidth="1"/>
+    <col min="11" max="11" width="8" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="64" t="s">
+        <v>256</v>
+      </c>
+      <c r="G7" s="64" t="s">
+        <v>180</v>
+      </c>
+      <c r="H7" s="64" t="s">
+        <v>181</v>
+      </c>
+      <c r="I7" s="64" t="s">
+        <v>182</v>
+      </c>
+      <c r="J7" s="64" t="s">
+        <v>183</v>
+      </c>
+      <c r="K7" s="64" t="s">
+        <v>184</v>
+      </c>
+      <c r="L7" s="64" t="s">
+        <v>202</v>
+      </c>
+      <c r="M7" s="64" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="23" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A8" s="75" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>257</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>257</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+    </row>
+    <row r="9" spans="1:13" s="23" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A9" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>261</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>261</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+    </row>
+    <row r="10" spans="1:13" s="23" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A10" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>262</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>262</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>260</v>
+      </c>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+    </row>
+    <row r="11" spans="1:13" s="23" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A11" s="75" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>290</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>290</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="37"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+    </row>
+    <row r="12" spans="1:13" s="72" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A12" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="76" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>272</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+    </row>
+    <row r="13" spans="1:13" ht="26.25">
+      <c r="A13" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="H13" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+    </row>
+    <row r="14" spans="1:13" ht="26.25">
+      <c r="A14" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>278</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+    </row>
+    <row r="15" spans="1:13" ht="26.25">
+      <c r="A15" s="75" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>283</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+    </row>
+    <row r="16" spans="1:13" ht="26.25">
+      <c r="A16" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>285</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>283</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+    </row>
+    <row r="17" spans="1:13" ht="28.5" customHeight="1">
+      <c r="A17" s="75" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>286</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>287</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>289</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>288</v>
+      </c>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="66"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="66"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>